<commit_message>
Updated format of sheet
</commit_message>
<xml_diff>
--- a/brinson_sheet.xlsx
+++ b/brinson_sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EYKS\Documents\UNDERGRADUATE\GHOSAL\PROGRAMMING\P&amp;L CALC, BRINSON PERFORMANCE EVALUATION\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EYKS\Documents\UNDERGRADUATE\GHOSAL\REPO\P&amp;L CALC, BRINSON PERFORMANCE EVALUATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16EE9969-9D8C-4596-9F03-893992CD5D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1FC3484-A55D-4A2C-BACA-DDC76F4E5A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{AE29B302-8747-49CE-9FC8-91D9627D1454}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>Portfolio weight</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Benchmark return</t>
   </si>
   <si>
-    <t>Factors</t>
-  </si>
-  <si>
     <t>USD</t>
   </si>
   <si>
@@ -89,13 +86,43 @@
     <t>Industrials</t>
   </si>
   <si>
-    <t>INDUSTRY</t>
-  </si>
-  <si>
-    <t>CURRENCY</t>
-  </si>
-  <si>
-    <t>COUNTRY</t>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Segments</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>CURRENCY AGGREGATE</t>
+  </si>
+  <si>
+    <t>INDUSTRY AGGREGATE</t>
+  </si>
+  <si>
+    <t>COUNTRY AGGREGATE</t>
   </si>
 </sst>
 </file>
@@ -456,44 +483,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1735D509-9C57-40ED-A7B6-5C5F5F6AAB22}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -504,13 +535,16 @@
       <c r="E2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -521,13 +555,16 @@
       <c r="E3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -538,13 +575,16 @@
       <c r="E4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -555,13 +595,16 @@
       <c r="E5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -572,13 +615,16 @@
       <c r="E6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -589,13 +635,16 @@
       <c r="E7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -606,13 +655,16 @@
       <c r="E8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -623,13 +675,16 @@
       <c r="E9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -640,13 +695,16 @@
       <c r="E10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -657,13 +715,16 @@
       <c r="E11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12">
-        <v>11</v>
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
       </c>
       <c r="C12">
         <v>11</v>
@@ -674,13 +735,16 @@
       <c r="E12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13">
-        <v>12</v>
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
       </c>
       <c r="C13">
         <v>12</v>
@@ -691,13 +755,16 @@
       <c r="E13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14">
-        <v>13</v>
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
       </c>
       <c r="C14">
         <v>13</v>
@@ -708,13 +775,16 @@
       <c r="E14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15">
-        <v>14</v>
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
       </c>
       <c r="C15">
         <v>14</v>
@@ -725,13 +795,16 @@
       <c r="E15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16">
-        <v>15</v>
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
       </c>
       <c r="C16">
         <v>15</v>
@@ -741,6 +814,110 @@
       </c>
       <c r="E16">
         <v>15</v>
+      </c>
+      <c r="F16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17">
+        <f>C16+1</f>
+        <v>16</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ref="D17:F20" si="0">D16+1</f>
+        <v>16</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18:C20" si="1">C17+1</f>
+        <v>17</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>